<commit_message>
updated DQBDD, combined results
</commit_message>
<xml_diff>
--- a/results/combinedresults/sat.xlsx
+++ b/results/combinedresults/sat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurajsic/OneDrive/skola/magisterFI/diplomka/DQBFbenchmarks/results/combinedresults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44E35DE-5AA7-DF41-8614-CAF09925AB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C75FDD2-8BE0-2749-8046-D7A68E61F306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15860" activeTab="1" xr2:uid="{093F9DC5-1B13-C14B-A0BF-58F8A491CE77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="42">
   <si>
     <t>tool</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>dCAQE 4.0.1</t>
+  </si>
+  <si>
+    <t>iProver v3.1 (CASC-27)</t>
+  </si>
+  <si>
+    <t>qbf-mode.SAT</t>
   </si>
 </sst>
 </file>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F5C62E-C27B-FB47-BBDD-61BAC8A1522B}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K3"/>
+      <selection activeCell="O1" sqref="O1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,7 +522,7 @@
     <col min="1" max="1" width="54.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +562,20 @@
       <c r="M1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -597,8 +615,20 @@
       <c r="M2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -638,8 +668,20 @@
       <c r="M3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -679,8 +721,20 @@
       <c r="M4">
         <v>9.6911360000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4">
+        <v>38.647736219999999</v>
+      </c>
+      <c r="P4">
+        <v>38.671415712684301</v>
+      </c>
+      <c r="Q4">
+        <v>120.844287999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -720,8 +774,20 @@
       <c r="M5">
         <v>30.519296000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5">
+        <v>564.51841155800003</v>
+      </c>
+      <c r="P5">
+        <v>564.13731784373499</v>
+      </c>
+      <c r="Q5">
+        <v>66.334719999999905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -761,8 +827,20 @@
       <c r="M6">
         <v>59.674624000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6">
+        <v>199.26957538799999</v>
+      </c>
+      <c r="P6">
+        <v>199.18121008202399</v>
+      </c>
+      <c r="Q6">
+        <v>112.336896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -802,8 +880,20 @@
       <c r="M7">
         <v>25.497599999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7">
+        <v>901.68943040500005</v>
+      </c>
+      <c r="P7">
+        <v>901.06485610827804</v>
+      </c>
+      <c r="Q7">
+        <v>100.306944</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -843,8 +933,20 @@
       <c r="M8">
         <v>44.232703999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8">
+        <v>901.684762761</v>
+      </c>
+      <c r="P8">
+        <v>901.065355155617</v>
+      </c>
+      <c r="Q8">
+        <v>46.534655999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -884,8 +986,20 @@
       <c r="M9">
         <v>35.92192</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9">
+        <v>901.68948187499996</v>
+      </c>
+      <c r="P9">
+        <v>901.03363374248102</v>
+      </c>
+      <c r="Q9">
+        <v>29.925376</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -925,8 +1039,20 @@
       <c r="M10">
         <v>60.243968000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10">
+        <v>901.69269355200004</v>
+      </c>
+      <c r="P10">
+        <v>901.04896248877003</v>
+      </c>
+      <c r="Q10">
+        <v>32.018431999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -966,8 +1092,20 @@
       <c r="M11">
         <v>60.600320000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11">
+        <v>901.59729099200001</v>
+      </c>
+      <c r="P11">
+        <v>901.04126202687598</v>
+      </c>
+      <c r="Q11">
+        <v>63.893504</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1007,8 +1145,20 @@
       <c r="M12">
         <v>70.750208000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12">
+        <v>901.69452224500003</v>
+      </c>
+      <c r="P12">
+        <v>901.05768045782997</v>
+      </c>
+      <c r="Q12">
+        <v>42.356735999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1048,8 +1198,20 @@
       <c r="M13">
         <v>42.979328000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13">
+        <v>901.68878475400004</v>
+      </c>
+      <c r="P13">
+        <v>901.04936884716096</v>
+      </c>
+      <c r="Q13">
+        <v>153.75564799999901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1089,8 +1251,20 @@
       <c r="M14">
         <v>53.170175999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14">
+        <v>901.68766515200002</v>
+      </c>
+      <c r="P14">
+        <v>901.049442827701</v>
+      </c>
+      <c r="Q14">
+        <v>48.336895999999903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1130,8 +1304,20 @@
       <c r="M15">
         <v>44.773375999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15">
+        <v>571.718645745</v>
+      </c>
+      <c r="P15">
+        <v>571.32172033190704</v>
+      </c>
+      <c r="Q15">
+        <v>139.03871999999899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1171,8 +1357,20 @@
       <c r="M16">
         <v>45.69088</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16">
+        <v>901.69762681700001</v>
+      </c>
+      <c r="P16">
+        <v>901.06158037111095</v>
+      </c>
+      <c r="Q16">
+        <v>87.478271999999905</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1212,8 +1410,20 @@
       <c r="M17">
         <v>40.730623999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17">
+        <v>901.59552580299999</v>
+      </c>
+      <c r="P17">
+        <v>901.06164992228105</v>
+      </c>
+      <c r="Q17">
+        <v>93.892607999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1253,8 +1463,20 @@
       <c r="M18">
         <v>47.681536000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18">
+        <v>901.69126809099998</v>
+      </c>
+      <c r="P18">
+        <v>901.05094260722399</v>
+      </c>
+      <c r="Q18">
+        <v>30.445567999999898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1294,8 +1516,20 @@
       <c r="M19">
         <v>44.6464</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19">
+        <v>901.69012872300004</v>
+      </c>
+      <c r="P19">
+        <v>901.06939081475105</v>
+      </c>
+      <c r="Q19">
+        <v>32.526336000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1335,8 +1569,20 @@
       <c r="M20">
         <v>44.613632000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20">
+        <v>901.69345665200001</v>
+      </c>
+      <c r="P20">
+        <v>901.04941850155501</v>
+      </c>
+      <c r="Q20">
+        <v>35.008511999999897</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1376,8 +1622,20 @@
       <c r="M21">
         <v>49.192959999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>36</v>
+      </c>
+      <c r="O21">
+        <v>901.69398287299998</v>
+      </c>
+      <c r="P21">
+        <v>901.04575139656595</v>
+      </c>
+      <c r="Q21">
+        <v>37.490687999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1417,8 +1675,20 @@
       <c r="M22">
         <v>56.262656</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22">
+        <v>901.69426082400003</v>
+      </c>
+      <c r="P22">
+        <v>901.04549301415602</v>
+      </c>
+      <c r="Q22">
+        <v>39.698431999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1458,8 +1728,20 @@
       <c r="M23">
         <v>51.912703999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23">
+        <v>901.58760404099996</v>
+      </c>
+      <c r="P23">
+        <v>901.06385182961799</v>
+      </c>
+      <c r="Q23">
+        <v>43.085823999999903</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1499,8 +1781,20 @@
       <c r="M24">
         <v>13.918208</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24">
+        <v>901.68764801299994</v>
+      </c>
+      <c r="P24">
+        <v>901.05780038237504</v>
+      </c>
+      <c r="Q24">
+        <v>36.237311999999903</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1539,6 +1833,18 @@
       </c>
       <c r="M25">
         <v>38.514688</v>
+      </c>
+      <c r="N25" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25">
+        <v>901.67430430800005</v>
+      </c>
+      <c r="P25">
+        <v>901.08178128674604</v>
+      </c>
+      <c r="Q25">
+        <v>59.908096</v>
       </c>
     </row>
   </sheetData>
@@ -1548,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15940F18-611E-B343-83C3-063D261F54BB}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1559,7 +1865,7 @@
     <col min="1" max="1" width="54.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1575,8 +1881,14 @@
       <c r="E1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1592,8 +1904,14 @@
       <c r="E2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1609,8 +1927,14 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1628,8 +1952,15 @@
         <f>runs!$C4+runs!$K4</f>
         <v>84.517844608999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <f>runs!$C4+runs!$O4</f>
+        <v>121.953791559</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1647,8 +1978,15 @@
         <f>runs!$C5+runs!$K5</f>
         <v>419.490098515</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <f>runs!$C5+runs!$O5</f>
+        <v>647.38832807300003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1666,8 +2004,15 @@
         <f>runs!$C6+runs!$K6</f>
         <v>139.24567262599999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <f>runs!$C6+runs!$O6</f>
+        <v>284.54559541399999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1685,8 +2030,15 @@
         <f>runs!$C7+runs!$K7</f>
         <v>147.492316743</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7">
+        <f>runs!$C7+runs!$O7</f>
+        <v>984.9101864480001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1704,8 +2056,15 @@
         <f>runs!$C8+runs!$K8</f>
         <v>985.42138445300009</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8">
+        <f>runs!$C8+runs!$O8</f>
+        <v>985.52727621400004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1723,8 +2082,15 @@
         <f>runs!$C9+runs!$K9</f>
         <v>983.39959418599994</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9">
+        <f>runs!$C9+runs!$O9</f>
+        <v>983.41400106099991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1742,8 +2108,15 @@
         <f>runs!$C10+runs!$K10</f>
         <v>1004.2402970400001</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10">
+        <f>runs!$C10+runs!$O10</f>
+        <v>1004.2567185920001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1761,8 +2134,15 @@
         <f>runs!$C11+runs!$K11</f>
         <v>985.52799491299993</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11">
+        <f>runs!$C11+runs!$O11</f>
+        <v>985.44300390500007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1780,8 +2160,15 @@
         <f>runs!$C12+runs!$K12</f>
         <v>1004.254336788</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12">
+        <f>runs!$C12+runs!$O12</f>
+        <v>1004.269619033</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1799,8 +2186,15 @@
         <f>runs!$C13+runs!$K13</f>
         <v>394.42028401100004</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13">
+        <f>runs!$C13+runs!$O13</f>
+        <v>987.027954765</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1818,8 +2212,15 @@
         <f>runs!$C14+runs!$K14</f>
         <v>964.08073540600003</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <f>runs!$C14+runs!$O14</f>
+        <v>964.18600255800004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1837,8 +2238,15 @@
         <f>runs!$C15+runs!$K15</f>
         <v>855.42918908299998</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15">
+        <f>runs!$C15+runs!$O15</f>
+        <v>652.40198882799996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1856,8 +2264,15 @@
         <f>runs!$C16+runs!$K16</f>
         <v>982.60770851099994</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16">
+        <f>runs!$C16+runs!$O16</f>
+        <v>982.624975328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1875,8 +2290,15 @@
         <f>runs!$C17+runs!$K17</f>
         <v>982.66458471199996</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17">
+        <f>runs!$C17+runs!$O17</f>
+        <v>982.58346451499995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1894,8 +2316,15 @@
         <f>runs!$C18+runs!$K18</f>
         <v>982.79798260000007</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18">
+        <f>runs!$C18+runs!$O18</f>
+        <v>982.81035669099992</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1913,8 +2342,15 @@
         <f>runs!$C19+runs!$K19</f>
         <v>982.95250367699998</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19">
+        <f>runs!$C19+runs!$O19</f>
+        <v>982.95435040000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1932,8 +2368,15 @@
         <f>runs!$C20+runs!$K20</f>
         <v>983.092790294</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20">
+        <f>runs!$C20+runs!$O20</f>
+        <v>983.10872894600004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1951,8 +2394,15 @@
         <f>runs!$C21+runs!$K21</f>
         <v>983.23247173300001</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21">
+        <f>runs!$C21+runs!$O21</f>
+        <v>983.34168560599994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1970,8 +2420,15 @@
         <f>runs!$C22+runs!$K22</f>
         <v>983.43518966400006</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22">
+        <f>runs!$C22+runs!$O22</f>
+        <v>983.45056248800006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1989,8 +2446,15 @@
         <f>runs!$C23+runs!$K23</f>
         <v>983.63426502300001</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23">
+        <f>runs!$C23+runs!$O23</f>
+        <v>983.54413306399999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2008,8 +2472,15 @@
         <f>runs!$C24+runs!$K24</f>
         <v>100.77277795900001</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24">
+        <f>runs!$C24+runs!$O24</f>
+        <v>982.43592217199989</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2027,8 +2498,15 @@
         <f>runs!$C25+runs!$K25</f>
         <v>963.23305273599999</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25">
+        <f>runs!$C25+runs!$O25</f>
+        <v>963.22285604400008</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2036,10 +2514,24 @@
         <f>COUNTIF(B4:B25,"sat") + COUNTIF(B4:B25,"unsat")</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f>COUNTIF(D4:D25,"sat") + COUNTIF(D4:D25,"unsat")</f>
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <f>COUNTIF(F4:F25,"sat") + COUNTIF(F4:F25,"unsat")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated combined results, added instances that dCAQE determines wrong result
</commit_message>
<xml_diff>
--- a/results/combinedresults/sat.xlsx
+++ b/results/combinedresults/sat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurajsic/OneDrive/skola/magisterFI/diplomka/DQBFbenchmarks/results/combinedresults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD95637-7E4C-AB49-817C-8FF322016941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E6BA9A-7695-EE41-B10F-8E282F290F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15860" activeTab="1" xr2:uid="{093F9DC5-1B13-C14B-A0BF-58F8A491CE77}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="53">
   <si>
     <t>tool</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>qbf-mode-noproofreconstruction.SAT</t>
   </si>
 </sst>
 </file>
@@ -546,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F5C62E-C27B-FB47-BBDD-61BAC8A1522B}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:X1048576"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,16 +682,16 @@
         <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="O2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="R2" t="s">
         <v>33</v>
@@ -848,10 +851,10 @@
         <v>34</v>
       </c>
       <c r="O4">
-        <v>38.647736219999999</v>
+        <v>38.873337665000001</v>
       </c>
       <c r="P4">
-        <v>38.671415712684301</v>
+        <v>38.877165973186401</v>
       </c>
       <c r="Q4">
         <v>120.844287999999</v>
@@ -931,13 +934,13 @@
         <v>35</v>
       </c>
       <c r="O5">
-        <v>564.51841155800003</v>
+        <v>210.39101399399999</v>
       </c>
       <c r="P5">
-        <v>564.13731784373499</v>
+        <v>210.26516573130999</v>
       </c>
       <c r="Q5">
-        <v>66.334719999999905</v>
+        <v>36.704256000000001</v>
       </c>
       <c r="R5" t="s">
         <v>36</v>
@@ -1014,13 +1017,13 @@
         <v>34</v>
       </c>
       <c r="O6">
-        <v>199.26957538799999</v>
+        <v>198.09790560499999</v>
       </c>
       <c r="P6">
-        <v>199.18121008202399</v>
+        <v>198.008979242295</v>
       </c>
       <c r="Q6">
-        <v>112.336896</v>
+        <v>112.332799999999</v>
       </c>
       <c r="R6" t="s">
         <v>34</v>
@@ -1094,16 +1097,16 @@
         <v>25.497599999999998</v>
       </c>
       <c r="N7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7">
-        <v>901.68943040500005</v>
+        <v>341.41489188700001</v>
       </c>
       <c r="P7">
-        <v>901.06485610827804</v>
+        <v>341.19318745285199</v>
       </c>
       <c r="Q7">
-        <v>100.306944</v>
+        <v>39.297024</v>
       </c>
       <c r="R7" t="s">
         <v>36</v>
@@ -1180,10 +1183,10 @@
         <v>36</v>
       </c>
       <c r="O8">
-        <v>901.684762761</v>
+        <v>901.69190069199999</v>
       </c>
       <c r="P8">
-        <v>901.065355155617</v>
+        <v>901.06110102310697</v>
       </c>
       <c r="Q8">
         <v>46.534655999999998</v>
@@ -1260,16 +1263,16 @@
         <v>35.92192</v>
       </c>
       <c r="N9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O9">
-        <v>901.68948187499996</v>
+        <v>364.90279952600002</v>
       </c>
       <c r="P9">
-        <v>901.03363374248102</v>
+        <v>364.66176222264698</v>
       </c>
       <c r="Q9">
-        <v>29.925376</v>
+        <v>22.990848</v>
       </c>
       <c r="R9" t="s">
         <v>35</v>
@@ -1346,13 +1349,13 @@
         <v>36</v>
       </c>
       <c r="O10">
-        <v>901.69269355200004</v>
+        <v>901.59020197200005</v>
       </c>
       <c r="P10">
-        <v>901.04896248877003</v>
+        <v>901.04938426241199</v>
       </c>
       <c r="Q10">
-        <v>32.018431999999997</v>
+        <v>32.014336</v>
       </c>
       <c r="R10" t="s">
         <v>36</v>
@@ -1429,13 +1432,13 @@
         <v>36</v>
       </c>
       <c r="O11">
-        <v>901.59729099200001</v>
+        <v>901.69378331799999</v>
       </c>
       <c r="P11">
-        <v>901.04126202687598</v>
+        <v>901.06163898110299</v>
       </c>
       <c r="Q11">
-        <v>63.893504</v>
+        <v>64.020479999999907</v>
       </c>
       <c r="R11" t="s">
         <v>36</v>
@@ -1512,13 +1515,13 @@
         <v>36</v>
       </c>
       <c r="O12">
-        <v>901.69452224500003</v>
+        <v>901.69429098000001</v>
       </c>
       <c r="P12">
-        <v>901.05768045782997</v>
+        <v>901.06575049832395</v>
       </c>
       <c r="Q12">
-        <v>42.356735999999998</v>
+        <v>42.352640000000001</v>
       </c>
       <c r="R12" t="s">
         <v>36</v>
@@ -1592,16 +1595,16 @@
         <v>42.979328000000002</v>
       </c>
       <c r="N13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O13">
-        <v>901.68878475400004</v>
+        <v>290.70346587900002</v>
       </c>
       <c r="P13">
-        <v>901.04936884716096</v>
+        <v>290.53796089067998</v>
       </c>
       <c r="Q13">
-        <v>153.75564799999901</v>
+        <v>47.423487999999999</v>
       </c>
       <c r="R13" t="s">
         <v>36</v>
@@ -1678,10 +1681,10 @@
         <v>36</v>
       </c>
       <c r="O14">
-        <v>901.68766515200002</v>
+        <v>901.69147759500004</v>
       </c>
       <c r="P14">
-        <v>901.049442827701</v>
+        <v>901.06580974906603</v>
       </c>
       <c r="Q14">
         <v>48.336895999999903</v>
@@ -1761,10 +1764,10 @@
         <v>34</v>
       </c>
       <c r="O15">
-        <v>571.718645745</v>
+        <v>570.91204480299996</v>
       </c>
       <c r="P15">
-        <v>571.32172033190704</v>
+        <v>570.50507144629898</v>
       </c>
       <c r="Q15">
         <v>139.03871999999899</v>
@@ -1844,10 +1847,10 @@
         <v>36</v>
       </c>
       <c r="O16">
-        <v>901.69762681700001</v>
+        <v>901.69746372500003</v>
       </c>
       <c r="P16">
-        <v>901.06158037111095</v>
+        <v>901.08165337145294</v>
       </c>
       <c r="Q16">
         <v>87.478271999999905</v>
@@ -1927,13 +1930,13 @@
         <v>36</v>
       </c>
       <c r="O17">
-        <v>901.59552580299999</v>
+        <v>901.593336357</v>
       </c>
       <c r="P17">
-        <v>901.06164992228105</v>
+        <v>901.04965047910798</v>
       </c>
       <c r="Q17">
-        <v>93.892607999999996</v>
+        <v>93.888511999999906</v>
       </c>
       <c r="R17" t="s">
         <v>36</v>
@@ -2010,13 +2013,13 @@
         <v>36</v>
       </c>
       <c r="O18">
-        <v>901.69126809099998</v>
+        <v>901.69411709600001</v>
       </c>
       <c r="P18">
-        <v>901.05094260722399</v>
+        <v>901.08165212720598</v>
       </c>
       <c r="Q18">
-        <v>30.445567999999898</v>
+        <v>30.441471999999901</v>
       </c>
       <c r="R18" t="s">
         <v>34</v>
@@ -2093,13 +2096,13 @@
         <v>36</v>
       </c>
       <c r="O19">
-        <v>901.69012872300004</v>
+        <v>901.69445660400004</v>
       </c>
       <c r="P19">
-        <v>901.06939081475105</v>
+        <v>901.04966185241904</v>
       </c>
       <c r="Q19">
-        <v>32.526336000000001</v>
+        <v>32.522239999999996</v>
       </c>
       <c r="R19" t="s">
         <v>36</v>
@@ -2176,10 +2179,10 @@
         <v>36</v>
       </c>
       <c r="O20">
-        <v>901.69345665200001</v>
+        <v>901.69414579700003</v>
       </c>
       <c r="P20">
-        <v>901.04941850155501</v>
+        <v>901.08171526342596</v>
       </c>
       <c r="Q20">
         <v>35.008511999999897</v>
@@ -2259,10 +2262,10 @@
         <v>36</v>
       </c>
       <c r="O21">
-        <v>901.69398287299998</v>
+        <v>901.68949501400004</v>
       </c>
       <c r="P21">
-        <v>901.04575139656595</v>
+        <v>901.04978442564595</v>
       </c>
       <c r="Q21">
         <v>37.490687999999999</v>
@@ -2342,10 +2345,10 @@
         <v>36</v>
       </c>
       <c r="O22">
-        <v>901.69426082400003</v>
+        <v>901.69221876899996</v>
       </c>
       <c r="P22">
-        <v>901.04549301415602</v>
+        <v>901.03381768241502</v>
       </c>
       <c r="Q22">
         <v>39.698431999999997</v>
@@ -2425,13 +2428,13 @@
         <v>36</v>
       </c>
       <c r="O23">
-        <v>901.58760404099996</v>
+        <v>901.57996135200005</v>
       </c>
       <c r="P23">
-        <v>901.06385182961799</v>
+        <v>901.038075443357</v>
       </c>
       <c r="Q23">
-        <v>43.085823999999903</v>
+        <v>43.081727999999998</v>
       </c>
       <c r="R23" t="s">
         <v>36</v>
@@ -2505,16 +2508,16 @@
         <v>13.918208</v>
       </c>
       <c r="N24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O24">
-        <v>901.68764801299994</v>
+        <v>582.11026493600002</v>
       </c>
       <c r="P24">
-        <v>901.05780038237504</v>
+        <v>581.70183198898997</v>
       </c>
       <c r="Q24">
-        <v>36.237311999999903</v>
+        <v>27.328512</v>
       </c>
       <c r="R24" t="s">
         <v>35</v>
@@ -2591,13 +2594,13 @@
         <v>36</v>
       </c>
       <c r="O25">
-        <v>901.67430430800005</v>
+        <v>901.67930187900004</v>
       </c>
       <c r="P25">
-        <v>901.08178128674604</v>
+        <v>901.06177636235896</v>
       </c>
       <c r="Q25">
-        <v>59.908096</v>
+        <v>59.903999999999897</v>
       </c>
       <c r="R25" t="s">
         <v>36</v>
@@ -2639,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15940F18-611E-B343-83C3-063D261F54BB}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2771,12 +2774,13 @@
         <f>runs!$C4+runs!$K4</f>
         <v>84.517844608999994</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
+      <c r="F4" t="str">
+        <f>runs!N4</f>
+        <v>sat</v>
       </c>
       <c r="G4">
         <f>runs!$C4+runs!$O4</f>
-        <v>121.953791559</v>
+        <v>122.17939300399999</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
@@ -2809,12 +2813,13 @@
         <f>runs!$C5+runs!$K5</f>
         <v>419.490098515</v>
       </c>
-      <c r="F5" t="s">
-        <v>35</v>
+      <c r="F5" t="str">
+        <f>runs!N5</f>
+        <v>unsat</v>
       </c>
       <c r="G5">
         <f>runs!$C5+runs!$O5</f>
-        <v>647.38832807300003</v>
+        <v>293.26093050899999</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -2847,12 +2852,13 @@
         <f>runs!$C6+runs!$K6</f>
         <v>139.24567262599999</v>
       </c>
-      <c r="F6" t="s">
-        <v>34</v>
+      <c r="F6" t="str">
+        <f>runs!N6</f>
+        <v>sat</v>
       </c>
       <c r="G6">
         <f>runs!$C6+runs!$O6</f>
-        <v>284.54559541399999</v>
+        <v>283.37392563100002</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -2885,12 +2891,13 @@
         <f>runs!$C7+runs!$K7</f>
         <v>147.492316743</v>
       </c>
-      <c r="F7" t="s">
-        <v>36</v>
+      <c r="F7" t="str">
+        <f>runs!N7</f>
+        <v>unsat</v>
       </c>
       <c r="G7">
         <f>runs!$C7+runs!$O7</f>
-        <v>984.9101864480001</v>
+        <v>424.63564793</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -2923,12 +2930,13 @@
         <f>runs!$C8+runs!$K8</f>
         <v>985.42138445300009</v>
       </c>
-      <c r="F8" t="s">
-        <v>36</v>
+      <c r="F8" t="str">
+        <f>runs!N8</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G8">
         <f>runs!$C8+runs!$O8</f>
-        <v>985.52727621400004</v>
+        <v>985.53441414500003</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -2961,12 +2969,13 @@
         <f>runs!$C9+runs!$K9</f>
         <v>983.39959418599994</v>
       </c>
-      <c r="F9" t="s">
-        <v>36</v>
+      <c r="F9" t="str">
+        <f>runs!N9</f>
+        <v>unsat</v>
       </c>
       <c r="G9">
         <f>runs!$C9+runs!$O9</f>
-        <v>983.41400106099991</v>
+        <v>446.62731871200003</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
@@ -2999,12 +3008,13 @@
         <f>runs!$C10+runs!$K10</f>
         <v>1004.2402970400001</v>
       </c>
-      <c r="F10" t="s">
-        <v>36</v>
+      <c r="F10" t="str">
+        <f>runs!N10</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G10">
         <f>runs!$C10+runs!$O10</f>
-        <v>1004.2567185920001</v>
+        <v>1004.1542270120001</v>
       </c>
       <c r="H10" t="s">
         <v>36</v>
@@ -3037,12 +3047,13 @@
         <f>runs!$C11+runs!$K11</f>
         <v>985.52799491299993</v>
       </c>
-      <c r="F11" t="s">
-        <v>36</v>
+      <c r="F11" t="str">
+        <f>runs!N11</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G11">
         <f>runs!$C11+runs!$O11</f>
-        <v>985.44300390500007</v>
+        <v>985.53949623099993</v>
       </c>
       <c r="H11" t="s">
         <v>36</v>
@@ -3075,12 +3086,13 @@
         <f>runs!$C12+runs!$K12</f>
         <v>1004.254336788</v>
       </c>
-      <c r="F12" t="s">
-        <v>36</v>
+      <c r="F12" t="str">
+        <f>runs!N12</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G12">
         <f>runs!$C12+runs!$O12</f>
-        <v>1004.269619033</v>
+        <v>1004.269387768</v>
       </c>
       <c r="H12" t="s">
         <v>36</v>
@@ -3113,12 +3125,13 @@
         <f>runs!$C13+runs!$K13</f>
         <v>394.42028401100004</v>
       </c>
-      <c r="F13" t="s">
-        <v>36</v>
+      <c r="F13" t="str">
+        <f>runs!N13</f>
+        <v>unsat</v>
       </c>
       <c r="G13">
         <f>runs!$C13+runs!$O13</f>
-        <v>987.027954765</v>
+        <v>376.04263589000004</v>
       </c>
       <c r="H13" t="s">
         <v>36</v>
@@ -3151,12 +3164,13 @@
         <f>runs!$C14+runs!$K14</f>
         <v>964.08073540600003</v>
       </c>
-      <c r="F14" t="s">
-        <v>36</v>
+      <c r="F14" t="str">
+        <f>runs!N14</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G14">
         <f>runs!$C14+runs!$O14</f>
-        <v>964.18600255800004</v>
+        <v>964.18981500100006</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -3189,12 +3203,13 @@
         <f>runs!$C15+runs!$K15</f>
         <v>855.42918908299998</v>
       </c>
-      <c r="F15" t="s">
-        <v>34</v>
+      <c r="F15" t="str">
+        <f>runs!N15</f>
+        <v>sat</v>
       </c>
       <c r="G15">
         <f>runs!$C15+runs!$O15</f>
-        <v>652.40198882799996</v>
+        <v>651.59538788599991</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -3227,12 +3242,13 @@
         <f>runs!$C16+runs!$K16</f>
         <v>982.60770851099994</v>
       </c>
-      <c r="F16" t="s">
-        <v>36</v>
+      <c r="F16" t="str">
+        <f>runs!N16</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G16">
         <f>runs!$C16+runs!$O16</f>
-        <v>982.624975328</v>
+        <v>982.62481223600003</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -3265,12 +3281,13 @@
         <f>runs!$C17+runs!$K17</f>
         <v>982.66458471199996</v>
       </c>
-      <c r="F17" t="s">
-        <v>36</v>
+      <c r="F17" t="str">
+        <f>runs!N17</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G17">
         <f>runs!$C17+runs!$O17</f>
-        <v>982.58346451499995</v>
+        <v>982.58127506899996</v>
       </c>
       <c r="H17" t="s">
         <v>36</v>
@@ -3303,12 +3320,13 @@
         <f>runs!$C18+runs!$K18</f>
         <v>982.79798260000007</v>
       </c>
-      <c r="F18" t="s">
-        <v>36</v>
+      <c r="F18" t="str">
+        <f>runs!N18</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G18">
         <f>runs!$C18+runs!$O18</f>
-        <v>982.81035669099992</v>
+        <v>982.81320569600007</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -3341,12 +3359,13 @@
         <f>runs!$C19+runs!$K19</f>
         <v>982.95250367699998</v>
       </c>
-      <c r="F19" t="s">
-        <v>36</v>
+      <c r="F19" t="str">
+        <f>runs!N19</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G19">
         <f>runs!$C19+runs!$O19</f>
-        <v>982.95435040000007</v>
+        <v>982.95867828100006</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -3379,12 +3398,13 @@
         <f>runs!$C20+runs!$K20</f>
         <v>983.092790294</v>
       </c>
-      <c r="F20" t="s">
-        <v>36</v>
+      <c r="F20" t="str">
+        <f>runs!N20</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G20">
         <f>runs!$C20+runs!$O20</f>
-        <v>983.10872894600004</v>
+        <v>983.10941809100007</v>
       </c>
       <c r="H20" t="s">
         <v>36</v>
@@ -3417,12 +3437,13 @@
         <f>runs!$C21+runs!$K21</f>
         <v>983.23247173300001</v>
       </c>
-      <c r="F21" t="s">
-        <v>36</v>
+      <c r="F21" t="str">
+        <f>runs!N21</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G21">
         <f>runs!$C21+runs!$O21</f>
-        <v>983.34168560599994</v>
+        <v>983.337197747</v>
       </c>
       <c r="H21" t="s">
         <v>36</v>
@@ -3455,12 +3476,13 @@
         <f>runs!$C22+runs!$K22</f>
         <v>983.43518966400006</v>
       </c>
-      <c r="F22" t="s">
-        <v>36</v>
+      <c r="F22" t="str">
+        <f>runs!N22</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G22">
         <f>runs!$C22+runs!$O22</f>
-        <v>983.45056248800006</v>
+        <v>983.448520433</v>
       </c>
       <c r="H22" t="s">
         <v>36</v>
@@ -3493,12 +3515,13 @@
         <f>runs!$C23+runs!$K23</f>
         <v>983.63426502300001</v>
       </c>
-      <c r="F23" t="s">
-        <v>36</v>
+      <c r="F23" t="str">
+        <f>runs!N23</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G23">
         <f>runs!$C23+runs!$O23</f>
-        <v>983.54413306399999</v>
+        <v>983.53649037500008</v>
       </c>
       <c r="H23" t="s">
         <v>36</v>
@@ -3531,12 +3554,13 @@
         <f>runs!$C24+runs!$K24</f>
         <v>100.77277795900001</v>
       </c>
-      <c r="F24" t="s">
-        <v>36</v>
+      <c r="F24" t="str">
+        <f>runs!N24</f>
+        <v>unsat</v>
       </c>
       <c r="G24">
         <f>runs!$C24+runs!$O24</f>
-        <v>982.43592217199989</v>
+        <v>662.85853909499997</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
@@ -3569,12 +3593,13 @@
         <f>runs!$C25+runs!$K25</f>
         <v>963.23305273599999</v>
       </c>
-      <c r="F25" t="s">
-        <v>36</v>
+      <c r="F25" t="str">
+        <f>runs!N25</f>
+        <v>TIMEOUT</v>
       </c>
       <c r="G25">
         <f>runs!$C25+runs!$O25</f>
-        <v>963.22285604400008</v>
+        <v>963.22785361500007</v>
       </c>
       <c r="H25" t="s">
         <v>36</v>
@@ -3615,7 +3640,7 @@
       </c>
       <c r="G27">
         <f xml:space="preserve"> SUMIF(F$4:F$25, "sat",G$4:G$25)</f>
-        <v>1058.9013758010001</v>
+        <v>1057.1487065209999</v>
       </c>
       <c r="H27">
         <f>COUNTIF(H$4:H$25,"sat")</f>
@@ -3656,11 +3681,11 @@
       </c>
       <c r="F28">
         <f>COUNTIF(F$4:F$25,"unsat")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <f xml:space="preserve"> SUMIF(F$4:F$25, "unsat",G$4:G$25)</f>
-        <v>647.38832807300003</v>
+        <v>2203.4250721360004</v>
       </c>
       <c r="H28">
         <f>COUNTIF(H$4:H$25,"unsat")</f>
@@ -3701,11 +3726,11 @@
       </c>
       <c r="F29">
         <f>COUNTIF(F$4:F$25,"sat") + COUNTIF(F$4:F$25,"unsat")</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G29">
         <f xml:space="preserve"> SUMIF(F$4:F$25, "sat",G$4:G$25)+ SUMIF(F$4:F$25, "unsat",G$4:G$25)</f>
-        <v>1706.2897038740002</v>
+        <v>3260.5737786570003</v>
       </c>
       <c r="H29">
         <f>COUNTIF(H$4:H$25,"sat") + COUNTIF(H$4:H$25,"unsat")</f>
@@ -3783,7 +3808,7 @@
       </c>
       <c r="F32">
         <f>COUNTIF(F$4:F$25,"TIMEOUT")</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H32">
         <f>COUNTIF(H$4:H$25,"TIMEOUT")</f>

</xml_diff>

<commit_message>
updated combined results for the newest HQS
</commit_message>
<xml_diff>
--- a/results/combinedresults/sat.xlsx
+++ b/results/combinedresults/sat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurajsic/OneDrive/vyzkum/dqbf/DQBFbenchmarks/results/combinedresults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812DE2EE-3772-844E-988E-5C1F5C7D5CA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BB44FC-7983-0F49-B3DE-A795DEA392C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{093F9DC5-1B13-C14B-A0BF-58F8A491CE77}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15780" activeTab="2" xr2:uid="{093F9DC5-1B13-C14B-A0BF-58F8A491CE77}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="realtime (sat2021paper)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'realtime (sat2021paper)'!$A$1:$K$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'realtime (sat2021paper)'!$A$1:$M$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'realtime (thesis)'!$A$1:$K$25</definedName>
     <definedName name="benchmark_hqs.2021_03_15_2006.results.SAT" localSheetId="0">runs!$AF$1:$AJ$25</definedName>
+    <definedName name="benchmark_hqs.2021_03_18_1932.results.SAT" localSheetId="0">runs!$AK$1:$AO$25</definedName>
     <definedName name="benchmark_iprover.2021_03_15_1800.results.qbf_mode_noproofreconstruction.SAT" localSheetId="0">runs!$AB$1:$AE$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -54,7 +55,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{E9B45343-3DF2-7E4B-8AE9-FC29467FC43C}" name="benchmark-iprover.2021-03-15_1800.results.qbf-mode-noproofreconstruction.SAT" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{5CCEDD4F-8E85-324E-B812-3DD189021D72}" name="benchmark-hqs.2021-03-18_1932.results.SAT" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/jurajsic/OneDrive/vyzkum/dqbf/DQBFbenchmarks/results/benchmark-hqs.2021-03-18_1932.results.SAT.csv" thousands=" ">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" xr16:uid="{E9B45343-3DF2-7E4B-8AE9-FC29467FC43C}" name="benchmark-iprover.2021-03-15_1800.results.qbf-mode-noproofreconstruction.SAT" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/jurajsic/OneDrive/vyzkum/dqbf/DQBFbenchmarks/results/benchmark-iprover.2021-03-15_1800.results.qbf-mode-noproofreconstruction.SAT.csv" thousands=" ">
       <textFields count="5">
         <textField/>
@@ -69,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="58">
   <si>
     <t>tool</t>
   </si>
@@ -235,6 +248,15 @@
   <si>
     <t>HQS 2 (2021-03-09)</t>
   </si>
+  <si>
+    <t>HQS 2 (2021-03-18)</t>
+  </si>
+  <si>
+    <t>uniquely solved (with older HQS)</t>
+  </si>
+  <si>
+    <t>uniquely solved (with newer HQS)</t>
+  </si>
 </sst>
 </file>
 
@@ -249,12 +271,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -269,8 +297,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -289,10 +318,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benchmark-iprover.2021-03-15_1800.results.qbf-mode-noproofreconstruction.SAT" connectionId="2" xr16:uid="{51D45A2C-77CF-184F-B651-A958E2C405C2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benchmark-hqs.2021-03-18_1932.results.SAT" connectionId="2" xr16:uid="{452194D2-48E1-FA4C-9655-7E6CF17C6A66}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benchmark-iprover.2021-03-15_1800.results.qbf-mode-noproofreconstruction.SAT" connectionId="3" xr16:uid="{51D45A2C-77CF-184F-B651-A958E2C405C2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="benchmark-hqs.2021-03-15_2006.results.SAT" connectionId="1" xr16:uid="{AB073F89-789C-A947-84E8-33DCFECEDC4B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -593,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F5C62E-C27B-FB47-BBDD-61BAC8A1522B}">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AN13" sqref="AN13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,9 +640,13 @@
     <col min="33" max="34" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -718,8 +755,23 @@
       <c r="AJ1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -828,8 +880,23 @@
       <c r="AJ2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -938,8 +1005,23 @@
       <c r="AJ3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1048,8 +1130,23 @@
       <c r="AJ4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL4">
+        <v>411.28142344299999</v>
+      </c>
+      <c r="AM4">
+        <v>411.01863977313002</v>
+      </c>
+      <c r="AN4">
+        <v>244.39193599999999</v>
+      </c>
+      <c r="AO4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1158,8 +1255,23 @@
       <c r="AJ5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL5">
+        <v>901.68162037000002</v>
+      </c>
+      <c r="AM5">
+        <v>901.05162827670495</v>
+      </c>
+      <c r="AN5">
+        <v>154.55027200000001</v>
+      </c>
+      <c r="AO5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1268,8 +1380,23 @@
       <c r="AJ6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL6">
+        <v>420.88149212000002</v>
+      </c>
+      <c r="AM6">
+        <v>420.633788436651</v>
+      </c>
+      <c r="AN6">
+        <v>183.88582399999899</v>
+      </c>
+      <c r="AO6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1378,8 +1505,23 @@
       <c r="AJ7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL7">
+        <v>901.68258537099996</v>
+      </c>
+      <c r="AM7">
+        <v>901.06553751975298</v>
+      </c>
+      <c r="AN7">
+        <v>156.70886400000001</v>
+      </c>
+      <c r="AO7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1488,8 +1630,23 @@
       <c r="AJ8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL8">
+        <v>901.588919777</v>
+      </c>
+      <c r="AM8">
+        <v>901.05747612565699</v>
+      </c>
+      <c r="AN8">
+        <v>232.58726399999901</v>
+      </c>
+      <c r="AO8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1598,8 +1755,23 @@
       <c r="AJ9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL9">
+        <v>901.67113507700003</v>
+      </c>
+      <c r="AM9">
+        <v>901.04910250753096</v>
+      </c>
+      <c r="AN9">
+        <v>132.636672</v>
+      </c>
+      <c r="AO9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1708,8 +1880,23 @@
       <c r="AJ10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL10">
+        <v>901.69113702000004</v>
+      </c>
+      <c r="AM10">
+        <v>901.06540778279305</v>
+      </c>
+      <c r="AN10">
+        <v>129.65887999999899</v>
+      </c>
+      <c r="AO10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1818,8 +2005,23 @@
       <c r="AJ11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL11">
+        <v>901.68007574000001</v>
+      </c>
+      <c r="AM11">
+        <v>901.06110119074503</v>
+      </c>
+      <c r="AN11">
+        <v>135.80287999999999</v>
+      </c>
+      <c r="AO11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1928,8 +2130,23 @@
       <c r="AJ12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL12">
+        <v>901.68529084700003</v>
+      </c>
+      <c r="AM12">
+        <v>901.08164553344204</v>
+      </c>
+      <c r="AN12">
+        <v>91.877375999999998</v>
+      </c>
+      <c r="AO12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2038,8 +2255,23 @@
       <c r="AJ13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL13">
+        <v>161.11702512400001</v>
+      </c>
+      <c r="AM13">
+        <v>161.041254080832</v>
+      </c>
+      <c r="AN13">
+        <v>90.243071999999998</v>
+      </c>
+      <c r="AO13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2148,8 +2380,23 @@
       <c r="AJ14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL14">
+        <v>901.59869353199997</v>
+      </c>
+      <c r="AM14">
+        <v>901.06496053934097</v>
+      </c>
+      <c r="AN14">
+        <v>139.681792</v>
+      </c>
+      <c r="AO14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2258,8 +2505,23 @@
       <c r="AJ15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL15">
+        <v>901.68136535300005</v>
+      </c>
+      <c r="AM15">
+        <v>901.04532205313399</v>
+      </c>
+      <c r="AN15">
+        <v>96.161791999999906</v>
+      </c>
+      <c r="AO15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2368,8 +2630,23 @@
       <c r="AJ16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL16">
+        <v>869.65303129699998</v>
+      </c>
+      <c r="AM16">
+        <v>869.06536335498095</v>
+      </c>
+      <c r="AN16">
+        <v>121.491456</v>
+      </c>
+      <c r="AO16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2478,8 +2755,23 @@
       <c r="AJ17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL17">
+        <v>901.68706554599999</v>
+      </c>
+      <c r="AM17">
+        <v>901.08160433918204</v>
+      </c>
+      <c r="AN17">
+        <v>123.83846399999899</v>
+      </c>
+      <c r="AO17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2588,8 +2880,23 @@
       <c r="AJ18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL18">
+        <v>901.68068892700001</v>
+      </c>
+      <c r="AM18">
+        <v>901.06511279195502</v>
+      </c>
+      <c r="AN18">
+        <v>129.74489599999899</v>
+      </c>
+      <c r="AO18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2698,8 +3005,23 @@
       <c r="AJ19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL19">
+        <v>901.68066157700002</v>
+      </c>
+      <c r="AM19">
+        <v>901.06573764979805</v>
+      </c>
+      <c r="AN19">
+        <v>123.387903999999</v>
+      </c>
+      <c r="AO19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2808,8 +3130,23 @@
       <c r="AJ20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL20">
+        <v>901.59101434599995</v>
+      </c>
+      <c r="AM20">
+        <v>901.02922515571095</v>
+      </c>
+      <c r="AN20">
+        <v>127.004672</v>
+      </c>
+      <c r="AO20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2918,8 +3255,23 @@
       <c r="AJ21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK21" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL21">
+        <v>901.68126990400003</v>
+      </c>
+      <c r="AM21">
+        <v>901.08130658417895</v>
+      </c>
+      <c r="AN21">
+        <v>130.42073600000001</v>
+      </c>
+      <c r="AO21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -3028,8 +3380,23 @@
       <c r="AJ22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL22">
+        <v>901.676364412</v>
+      </c>
+      <c r="AM22">
+        <v>901.04968257248402</v>
+      </c>
+      <c r="AN22">
+        <v>128.70041599999999</v>
+      </c>
+      <c r="AO22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3138,8 +3505,23 @@
       <c r="AJ23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL23">
+        <v>901.68464145300004</v>
+      </c>
+      <c r="AM23">
+        <v>901.06579589098601</v>
+      </c>
+      <c r="AN23">
+        <v>129.24518399999999</v>
+      </c>
+      <c r="AO23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3248,8 +3630,23 @@
       <c r="AJ24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL24">
+        <v>901.67459146800002</v>
+      </c>
+      <c r="AM24">
+        <v>901.06502982228994</v>
+      </c>
+      <c r="AN24">
+        <v>144.90419199999999</v>
+      </c>
+      <c r="AO24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3356,6 +3753,21 @@
         <v>171.78623999999999</v>
       </c>
       <c r="AJ25" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL25">
+        <v>901.67836040500003</v>
+      </c>
+      <c r="AM25">
+        <v>901.08116213977303</v>
+      </c>
+      <c r="AN25">
+        <v>178.733056</v>
+      </c>
+      <c r="AO25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4578,18 +4990,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8BA565-CB29-DF41-86C0-325693778015}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4623,8 +5037,14 @@
       <c r="K1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4658,8 +5078,14 @@
       <c r="K2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4693,8 +5119,14 @@
       <c r="K3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4734,8 +5166,14 @@
       <c r="K4">
         <v>901.68752353000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4">
+        <v>411.28142344299999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4775,8 +5213,14 @@
       <c r="K5">
         <v>901.68960319099995</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5">
+        <v>901.68162037000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4816,8 +5260,14 @@
       <c r="K6">
         <v>901.67721245400003</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6">
+        <v>420.88149212000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4857,8 +5307,14 @@
       <c r="K7">
         <v>901.59191515400005</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7">
+        <v>901.68258537099996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4898,8 +5354,14 @@
       <c r="K8">
         <v>901.69223948199999</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8">
+        <v>901.588919777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4939,8 +5401,14 @@
       <c r="K9">
         <v>901.70783484900005</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9">
+        <v>901.67113507700003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4980,8 +5448,14 @@
       <c r="K10">
         <v>901.68435881200003</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10">
+        <v>901.69113702000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -5021,8 +5495,14 @@
       <c r="K11">
         <v>901.72287170499999</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11">
+        <v>901.68007574000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -5062,8 +5542,14 @@
       <c r="K12">
         <v>901.67789361099994</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12">
+        <v>901.68529084700003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -5103,8 +5589,14 @@
       <c r="K13">
         <v>901.58992234699997</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13">
+        <v>161.11702512400001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5144,8 +5636,14 @@
       <c r="K14">
         <v>100.23334106199999</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14">
+        <v>901.59869353199997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -5185,8 +5683,14 @@
       <c r="K15">
         <v>901.68927400400003</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15">
+        <v>901.68136535300005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -5226,8 +5730,14 @@
       <c r="K16">
         <v>901.68209472700005</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16">
+        <v>869.65303129699998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -5267,8 +5777,14 @@
       <c r="K17">
         <v>901.69477151900003</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17">
+        <v>901.68706554599999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -5308,8 +5824,14 @@
       <c r="K18">
         <v>901.67485828500003</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18">
+        <v>901.68068892700001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -5349,8 +5871,14 @@
       <c r="K19">
         <v>901.58268729899999</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19">
+        <v>901.68066157700002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -5390,8 +5918,14 @@
       <c r="K20">
         <v>901.68978389999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20">
+        <v>901.59101434599995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -5431,8 +5965,14 @@
       <c r="K21">
         <v>901.68064061300004</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21">
+        <v>901.68126990400003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -5472,8 +6012,14 @@
       <c r="K22">
         <v>901.68176643000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22">
+        <v>901.676364412</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -5513,8 +6059,14 @@
       <c r="K23">
         <v>901.69052446000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23">
+        <v>901.68464145300004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -5554,8 +6106,14 @@
       <c r="K24">
         <v>122.45577283</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M24">
+        <v>901.67459146800002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -5595,8 +6153,14 @@
       <c r="K25">
         <v>101.845925041</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25">
+        <v>901.67836040500003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -5640,8 +6204,16 @@
         <f xml:space="preserve"> SUMIF(J$4:J$25, "sat",K$4:K$25)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f>COUNTIF(L$4:L$25,"sat")</f>
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <f xml:space="preserve"> SUMIF(L$4:L$25, "sat",M$4:M$25)</f>
+        <v>1701.8159468600002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -5685,8 +6257,16 @@
         <f xml:space="preserve"> SUMIF(J$4:J$25, "unsat",K$4:K$25)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f>COUNTIF(L$4:L$25,"unsat")</f>
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <f xml:space="preserve"> SUMIF(L$4:L$25, "unsat",M$4:M$25)</f>
+        <v>161.11702512400001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -5730,10 +6310,18 @@
         <f xml:space="preserve"> SUMIF(J$4:J$25, "sat",K$4:K$25)+ SUMIF(J$4:J$25, "unsat",K$4:K$25)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <f>COUNTIF(L$4:L$25,"sat") + COUNTIF(L$4:L$25,"unsat")</f>
+        <v>4</v>
+      </c>
+      <c r="M29">
+        <f xml:space="preserve"> SUMIF(L$4:L$25, "sat",M$4:M$25)+ SUMIF(L$4:L$25, "unsat",M$4:M$25)</f>
+        <v>1862.9329719840002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -5744,90 +6332,126 @@
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
       <c r="J30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>48</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <f>COUNTIF(B$4:B$25,"OUT OF MEMORY")</f>
         <v>0</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <f>COUNTIF(D$4:D$25,"OUT OF MEMORY")</f>
         <v>0</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <f>COUNTIF(F$4:F$25,"OUT OF MEMORY")</f>
         <v>0</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <f>COUNTIF(H$4:H$25,"OUT OF MEMORY")</f>
         <v>0</v>
       </c>
-      <c r="J31">
+      <c r="J32">
         <f>COUNTIF(J$4:J$25,"OUT OF MEMORY")</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="L32">
+        <f>COUNTIF(L$4:L$25,"OUT OF MEMORY")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>49</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <f>COUNTIF(B$4:B$25,"TIMEOUT")</f>
         <v>13</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <f>COUNTIF(D$4:D$25,"TIMEOUT")</f>
         <v>15</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <f>COUNTIF(F$4:F$25,"TIMEOUT")</f>
         <v>14</v>
       </c>
-      <c r="H32">
+      <c r="H33">
         <f>COUNTIF(H$4:H$25,"TIMEOUT")</f>
         <v>18</v>
       </c>
-      <c r="J32">
+      <c r="J33">
         <f>COUNTIF(J$4:J$25,"TIMEOUT")</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="L33">
+        <f>COUNTIF(L$4:L$25,"TIMEOUT")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>50</v>
       </c>
-      <c r="B33">
-        <f>22-B29-B31-B32</f>
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <f>22-D29-D31-D32</f>
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <f>22-F29-F31-F32</f>
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <f>22-H29-H31-H32</f>
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <f>22-J29-J31-J32</f>
+      <c r="B34">
+        <f>22-B29-B32-B33</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f>22-D29-D32-D33</f>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f>22-F29-F32-F33</f>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f>22-H29-H32-H33</f>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f>22-J29-J32-J33</f>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f>22-L29-L32-L33</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K25" xr:uid="{7BA85B73-FD3C-5048-9A1A-966612B6D032}"/>
+  <autoFilter ref="A1:M25" xr:uid="{AC914079-61A2-314D-856B-7A0B32EC8DAB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>